<commit_message>
Minor updates to various files
</commit_message>
<xml_diff>
--- a/data/cas_errors.xlsx
+++ b/data/cas_errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIVER37\Documents\casfri\cas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C02C61-A144-4E3A-86AB-77B721553771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5920D2-7CA2-4A42-BE05-D3911930FF23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="168">
   <si>
     <t>Class</t>
   </si>
@@ -509,13 +509,22 @@
     <t>Geometry</t>
   </si>
   <si>
-    <t>NULL_EQUIV</t>
-  </si>
-  <si>
-    <t>Null equivalent</t>
-  </si>
-  <si>
     <t>INVALID_VALUE</t>
+  </si>
+  <si>
+    <t>Unknown value</t>
+  </si>
+  <si>
+    <t>UNKNOWN_VALUE</t>
+  </si>
+  <si>
+    <t>PHOTO_YEAR in AB</t>
+  </si>
+  <si>
+    <t>Unknow_value</t>
+  </si>
+  <si>
+    <t>UNKNOW_VALUE</t>
   </si>
 </sst>
 </file>
@@ -1378,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1460,36 +1469,36 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2">
-        <v>-8888</v>
+        <v>-8889</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2">
-        <v>-8889</v>
+        <v>-8888</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1510,168 +1519,173 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="8">
+        <v>-8886</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="6">
+        <v>-8885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G9" s="2">
         <v>-9999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2">
-        <v>-9998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" s="2">
-        <v>-9997</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G10" s="2">
-        <v>-9996</v>
+        <v>-9998</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-9997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-9996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F13" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G13" s="2">
         <v>-9995</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G14" s="2">
         <v>-3333</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>161</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>155</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>158</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G15" s="2">
         <v>-7779</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>156</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>157</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>160</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G16" s="2">
         <v>-7778</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="G16" s="8">
-        <v>-8886</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G17" s="6">
-        <v>-8889</v>
       </c>
     </row>
   </sheetData>
@@ -1682,11 +1696,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1695,16 +1709,17 @@
     <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.09765625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.69921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>64</v>
       </c>
@@ -1718,28 +1733,31 @@
         <v>146</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -1758,9 +1776,6 @@
       <c r="F2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
@@ -1773,8 +1788,11 @@
       <c r="K2" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>67</v>
       </c>
@@ -1790,9 +1808,6 @@
       <c r="F3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1805,8 +1820,11 @@
       <c r="K3" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>68</v>
       </c>
@@ -1822,9 +1840,6 @@
       <c r="F4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1837,8 +1852,11 @@
       <c r="K4" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>69</v>
       </c>
@@ -1854,9 +1872,6 @@
       <c r="F5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
@@ -1869,8 +1884,11 @@
       <c r="K5" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>70</v>
       </c>
@@ -1881,14 +1899,11 @@
         <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H6" s="2" t="s">
         <v>45</v>
       </c>
@@ -1896,13 +1911,16 @@
         <v>45</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>71</v>
       </c>
@@ -1918,9 +1936,6 @@
       <c r="F7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H7" s="2" t="s">
         <v>45</v>
       </c>
@@ -1933,8 +1948,11 @@
       <c r="K7" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>72</v>
       </c>
@@ -1945,14 +1963,11 @@
         <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H8" s="2" t="s">
         <v>45</v>
       </c>
@@ -1960,13 +1975,16 @@
         <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>73</v>
       </c>
@@ -1982,9 +2000,6 @@
       <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H9" s="2" t="s">
         <v>45</v>
       </c>
@@ -1997,8 +2012,11 @@
       <c r="K9" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>74</v>
       </c>
@@ -2014,9 +2032,6 @@
       <c r="F10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H10" s="2" t="s">
         <v>45</v>
       </c>
@@ -2029,8 +2044,11 @@
       <c r="K10" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>75</v>
       </c>
@@ -2046,9 +2064,6 @@
       <c r="F11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H11" s="2" t="s">
         <v>45</v>
       </c>
@@ -2061,8 +2076,11 @@
       <c r="K11" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>76</v>
       </c>
@@ -2078,9 +2096,6 @@
       <c r="F12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H12" s="2" t="s">
         <v>45</v>
       </c>
@@ -2093,8 +2108,11 @@
       <c r="K12" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>77</v>
       </c>
@@ -2110,9 +2128,6 @@
       <c r="F13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H13" s="2" t="s">
         <v>45</v>
       </c>
@@ -2123,10 +2138,13 @@
         <v>45</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>78</v>
       </c>
@@ -2142,9 +2160,6 @@
       <c r="F14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H14" s="2" t="s">
         <v>45</v>
       </c>
@@ -2157,8 +2172,11 @@
       <c r="K14" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -2174,9 +2192,6 @@
       <c r="F15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H15" s="2" t="s">
         <v>45</v>
       </c>
@@ -2189,8 +2204,11 @@
       <c r="K15" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>80</v>
       </c>
@@ -2206,9 +2224,6 @@
       <c r="F16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H16" s="2" t="s">
         <v>45</v>
       </c>
@@ -2221,8 +2236,11 @@
       <c r="K16" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>81</v>
       </c>
@@ -2238,9 +2256,6 @@
       <c r="F17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H17" s="2" t="s">
         <v>45</v>
       </c>
@@ -2253,8 +2268,11 @@
       <c r="K17" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>82</v>
       </c>
@@ -2270,9 +2288,6 @@
       <c r="F18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H18" s="2" t="s">
         <v>45</v>
       </c>
@@ -2285,8 +2300,11 @@
       <c r="K18" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>83</v>
       </c>
@@ -2296,29 +2314,29 @@
       <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="2">
         <v>-8888</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="2">
         <v>-9998</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>84</v>
       </c>
@@ -2328,29 +2346,29 @@
       <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="2">
         <v>-8888</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="2">
         <v>-9998</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -2364,14 +2382,11 @@
         <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H21" s="2" t="s">
         <v>45</v>
       </c>
@@ -2384,8 +2399,11 @@
       <c r="K21" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>86</v>
       </c>
@@ -2396,28 +2414,28 @@
         <v>39</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K22" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>87</v>
       </c>
@@ -2433,9 +2451,6 @@
       <c r="F23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H23" s="2" t="s">
         <v>45</v>
       </c>
@@ -2446,10 +2461,13 @@
         <v>45</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>88</v>
       </c>
@@ -2465,9 +2483,6 @@
       <c r="F24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2480,8 +2495,11 @@
       <c r="K24" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>89</v>
       </c>
@@ -2491,29 +2509,29 @@
       <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="2">
         <v>-8888</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="2">
         <v>-9998</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>90</v>
       </c>
@@ -2524,14 +2542,11 @@
         <v>45</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H26" s="2" t="s">
         <v>45</v>
       </c>
@@ -2544,8 +2559,11 @@
       <c r="K26" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>91</v>
       </c>
@@ -2555,29 +2573,29 @@
       <c r="D27" s="2">
         <v>-9995</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="2">
         <v>-8888</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="2">
         <v>-9999</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K27" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>92</v>
       </c>
@@ -2587,29 +2605,29 @@
       <c r="D28" s="2">
         <v>-9995</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="2">
         <v>-8888</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="2">
         <v>-9999</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K28" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>93</v>
       </c>
@@ -2619,29 +2637,29 @@
       <c r="D29" s="2">
         <v>-9995</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="2">
         <v>-8888</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="2">
         <v>-9999</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K29" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>94</v>
       </c>
@@ -2651,29 +2669,32 @@
       <c r="D30" s="2">
         <v>-9995</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="2">
         <v>-8888</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="G30" s="2" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" s="2">
         <v>-9999</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K30" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2687,14 +2708,11 @@
         <v>45</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H31" s="2" t="s">
         <v>45</v>
       </c>
@@ -2707,8 +2725,11 @@
       <c r="K31" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>46</v>
       </c>
@@ -2719,14 +2740,11 @@
         <v>45</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H32" s="2" t="s">
         <v>45</v>
       </c>
@@ -2734,13 +2752,16 @@
         <v>45</v>
       </c>
       <c r="J32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -2756,23 +2777,23 @@
       <c r="F33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="2">
+      <c r="H33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="2">
         <v>-8887</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J33" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>48</v>
       </c>
@@ -2788,9 +2809,6 @@
       <c r="F34" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H34" s="2" t="s">
         <v>45</v>
       </c>
@@ -2803,8 +2821,11 @@
       <c r="K34" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>49</v>
       </c>
@@ -2820,9 +2841,6 @@
       <c r="F35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H35" s="2" t="s">
         <v>45</v>
       </c>
@@ -2835,8 +2853,11 @@
       <c r="K35" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -2846,29 +2867,29 @@
       <c r="D36" s="2">
         <v>-9995</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="2">
         <v>-8888</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="2">
         <v>-9999</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K36" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>51</v>
       </c>
@@ -2878,29 +2899,29 @@
       <c r="D37" s="2">
         <v>-9995</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="2">
         <v>-8888</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="2">
         <v>-9999</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K37" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>52</v>
       </c>
@@ -2910,29 +2931,29 @@
       <c r="D38" s="2">
         <v>-9995</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="2">
         <v>-8888</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J38" s="2">
         <v>-9999</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K38" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L38" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>53</v>
       </c>
@@ -2942,29 +2963,29 @@
       <c r="D39" s="2">
         <v>-9995</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="2">
         <v>-8888</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" s="2">
         <v>-9999</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K39" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>54</v>
       </c>
@@ -2975,14 +2996,11 @@
         <v>45</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H40" s="2" t="s">
         <v>45</v>
       </c>
@@ -2990,13 +3008,16 @@
         <v>45</v>
       </c>
       <c r="J40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K40" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>116</v>
       </c>
@@ -3007,28 +3028,28 @@
         <v>45</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K41" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>117</v>
       </c>
@@ -3038,29 +3059,29 @@
       <c r="D42" s="2">
         <v>-9995</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="2">
         <v>-8888</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H42" s="2">
+      <c r="H42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="2">
         <v>-8887</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>-9999</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K42" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>118</v>
       </c>
@@ -3071,28 +3092,28 @@
         <v>45</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L43" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>119</v>
       </c>
@@ -3102,29 +3123,29 @@
       <c r="D44" s="2">
         <v>-9995</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="2">
         <v>-8888</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H44" s="2">
+      <c r="H44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="2">
         <v>-8887</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>-9999</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K44" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L44" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>120</v>
       </c>
@@ -3135,28 +3156,28 @@
         <v>45</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K45" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L45" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>121</v>
       </c>
@@ -3166,29 +3187,29 @@
       <c r="D46" s="2">
         <v>-9995</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="2">
         <v>-8888</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" s="2">
+      <c r="H46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I46" s="2">
         <v>-8887</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>-9999</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K46" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>122</v>
       </c>
@@ -3199,28 +3220,28 @@
         <v>45</v>
       </c>
       <c r="E47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K47" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K47" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L47" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>123</v>
       </c>
@@ -3230,29 +3251,29 @@
       <c r="D48" s="2">
         <v>-9995</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="2">
         <v>-8888</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H48" s="2">
+      <c r="H48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I48" s="2">
         <v>-8887</v>
       </c>
-      <c r="I48" s="2">
+      <c r="J48" s="2">
         <v>-9999</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K48" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L48" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>124</v>
       </c>
@@ -3263,28 +3284,28 @@
         <v>45</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K49" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L49" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>125</v>
       </c>
@@ -3294,29 +3315,29 @@
       <c r="D50" s="2">
         <v>-9995</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="2">
         <v>-8888</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H50" s="2">
+      <c r="H50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I50" s="2">
         <v>-8887</v>
       </c>
-      <c r="I50" s="2">
+      <c r="J50" s="2">
         <v>-9999</v>
       </c>
-      <c r="J50" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K50" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L50" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>126</v>
       </c>
@@ -3327,28 +3348,28 @@
         <v>45</v>
       </c>
       <c r="E51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K51" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L51" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>127</v>
       </c>
@@ -3358,29 +3379,29 @@
       <c r="D52" s="2">
         <v>-9995</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="2">
         <v>-8888</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" s="2">
+      <c r="H52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="2">
         <v>-8887</v>
       </c>
-      <c r="I52" s="2">
+      <c r="J52" s="2">
         <v>-9999</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K52" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>128</v>
       </c>
@@ -3391,28 +3412,28 @@
         <v>45</v>
       </c>
       <c r="E53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K53" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K53" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L53" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>129</v>
       </c>
@@ -3422,29 +3443,29 @@
       <c r="D54" s="2">
         <v>-9995</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" s="2">
         <v>-8888</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H54" s="2">
+      <c r="H54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I54" s="2">
         <v>-8887</v>
       </c>
-      <c r="I54" s="2">
+      <c r="J54" s="2">
         <v>-9999</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K54" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>130</v>
       </c>
@@ -3455,28 +3476,28 @@
         <v>45</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K55" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K55" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>131</v>
       </c>
@@ -3486,29 +3507,29 @@
       <c r="D56" s="2">
         <v>-9995</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="2">
         <v>-8888</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H56" s="2">
+      <c r="H56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I56" s="2">
         <v>-8887</v>
       </c>
-      <c r="I56" s="2">
+      <c r="J56" s="2">
         <v>-9999</v>
       </c>
-      <c r="J56" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K56" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>132</v>
       </c>
@@ -3519,28 +3540,28 @@
         <v>45</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I57" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K57" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>133</v>
       </c>
@@ -3550,29 +3571,29 @@
       <c r="D58" s="2">
         <v>-9995</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" s="2">
         <v>-8888</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H58" s="2">
+      <c r="H58" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I58" s="2">
         <v>-8887</v>
       </c>
-      <c r="I58" s="2">
+      <c r="J58" s="2">
         <v>-9999</v>
       </c>
-      <c r="J58" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K58" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>134</v>
       </c>
@@ -3583,28 +3604,28 @@
         <v>45</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K59" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K59" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>135</v>
       </c>
@@ -3614,29 +3635,29 @@
       <c r="D60" s="2">
         <v>-9995</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="2">
         <v>-8888</v>
       </c>
-      <c r="F60" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H60" s="2">
+      <c r="H60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I60" s="2">
         <v>-8887</v>
       </c>
-      <c r="I60" s="2">
+      <c r="J60" s="2">
         <v>-9999</v>
       </c>
-      <c r="J60" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K60" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L60" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>55</v>
       </c>
@@ -3647,28 +3668,28 @@
         <v>-9995</v>
       </c>
       <c r="E61" s="2">
+        <v>-8886</v>
+      </c>
+      <c r="F61" s="2">
         <v>-8888</v>
       </c>
-      <c r="F61" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H61" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J61" s="2">
         <v>-9999</v>
       </c>
-      <c r="J61" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K61" s="2">
+      <c r="K61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L61" s="2">
         <v>-9997</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>56</v>
       </c>
@@ -3679,28 +3700,28 @@
         <v>-9995</v>
       </c>
       <c r="E62" s="2">
+        <v>-8886</v>
+      </c>
+      <c r="F62" s="2">
         <v>-8888</v>
       </c>
-      <c r="F62" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H62" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J62" s="2">
         <v>-9999</v>
       </c>
-      <c r="J62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K62" s="2">
+      <c r="K62" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L62" s="2">
         <v>-9997</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>57</v>
       </c>
@@ -3716,23 +3737,23 @@
       <c r="F63" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H63" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I63" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J63" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L63" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>58</v>
       </c>
@@ -3748,9 +3769,6 @@
       <c r="F64" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H64" s="2" t="s">
         <v>45</v>
       </c>
@@ -3760,11 +3778,14 @@
       <c r="J64" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L64" s="2">
         <v>-9997</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>113</v>
       </c>
@@ -3778,14 +3799,11 @@
         <v>45</v>
       </c>
       <c r="E65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H65" s="2" t="s">
         <v>45</v>
       </c>
@@ -3798,8 +3816,11 @@
       <c r="K65" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>46</v>
       </c>
@@ -3810,14 +3831,11 @@
         <v>45</v>
       </c>
       <c r="E66" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H66" s="2" t="s">
         <v>45</v>
       </c>
@@ -3825,13 +3843,16 @@
         <v>45</v>
       </c>
       <c r="J66" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K66" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>47</v>
       </c>
@@ -3847,23 +3868,23 @@
       <c r="F67" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H67" s="2">
+      <c r="H67" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I67" s="2">
         <v>-8887</v>
       </c>
-      <c r="I67" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J67" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>48</v>
       </c>
@@ -3879,9 +3900,6 @@
       <c r="F68" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G68" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H68" s="2" t="s">
         <v>45</v>
       </c>
@@ -3894,8 +3912,11 @@
       <c r="K68" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>49</v>
       </c>
@@ -3911,9 +3932,6 @@
       <c r="F69" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H69" s="2" t="s">
         <v>45</v>
       </c>
@@ -3926,8 +3944,11 @@
       <c r="K69" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>51</v>
       </c>
@@ -3937,29 +3958,29 @@
       <c r="D70" s="2">
         <v>-9995</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" s="2">
         <v>-8888</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H70" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I70" s="2">
+      <c r="I70" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J70" s="2">
         <v>-9999</v>
       </c>
-      <c r="J70" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K70" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>50</v>
       </c>
@@ -3969,29 +3990,29 @@
       <c r="D71" s="2">
         <v>-9995</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" s="2">
         <v>-8888</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H71" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I71" s="2">
+      <c r="I71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J71" s="2">
         <v>-9999</v>
       </c>
-      <c r="J71" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K71" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>53</v>
       </c>
@@ -4001,29 +4022,29 @@
       <c r="D72" s="2">
         <v>-9995</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F72" s="2">
         <v>-8888</v>
       </c>
-      <c r="F72" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H72" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I72" s="2">
+      <c r="I72" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J72" s="2">
         <v>-9999</v>
       </c>
-      <c r="J72" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K72" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>52</v>
       </c>
@@ -4033,29 +4054,29 @@
       <c r="D73" s="2">
         <v>-9995</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" s="2">
         <v>-8888</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H73" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I73" s="2">
+      <c r="I73" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J73" s="2">
         <v>-9999</v>
       </c>
-      <c r="J73" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K73" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>59</v>
       </c>
@@ -4066,14 +4087,11 @@
         <v>45</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H74" s="2" t="s">
         <v>45</v>
       </c>
@@ -4086,8 +4104,11 @@
       <c r="K74" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>60</v>
       </c>
@@ -4098,14 +4119,11 @@
         <v>45</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H75" s="2" t="s">
         <v>45</v>
       </c>
@@ -4116,10 +4134,13 @@
         <v>45</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>61</v>
       </c>
@@ -4130,14 +4151,11 @@
         <v>45</v>
       </c>
       <c r="E76" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H76" s="2" t="s">
         <v>45</v>
       </c>
@@ -4150,8 +4168,11 @@
       <c r="K76" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>114</v>
       </c>
@@ -4165,14 +4186,11 @@
         <v>45</v>
       </c>
       <c r="E77" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H77" s="2" t="s">
         <v>45</v>
       </c>
@@ -4185,8 +4203,11 @@
       <c r="K77" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L77" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>96</v>
       </c>
@@ -4197,14 +4218,11 @@
         <v>45</v>
       </c>
       <c r="E78" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H78" s="2" t="s">
         <v>45</v>
       </c>
@@ -4212,13 +4230,16 @@
         <v>45</v>
       </c>
       <c r="J78" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K78" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K78" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>98</v>
       </c>
@@ -4228,29 +4249,29 @@
       <c r="D79" s="2">
         <v>-9995</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" s="2">
         <v>-8888</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H79" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I79" s="2">
+      <c r="I79" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J79" s="2">
         <v>-9999</v>
       </c>
-      <c r="J79" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K79" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>100</v>
       </c>
@@ -4261,28 +4282,28 @@
         <v>-9995</v>
       </c>
       <c r="E80" s="2">
+        <v>-8885</v>
+      </c>
+      <c r="F80" s="2">
         <v>-8888</v>
       </c>
-      <c r="F80" s="2">
-        <v>-8885</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H80" s="2">
+      <c r="H80" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I80" s="2">
         <v>-8887</v>
       </c>
-      <c r="I80" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J80" s="2">
+      <c r="J80" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K80" s="2">
         <v>-9998</v>
       </c>
-      <c r="K80" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>102</v>
       </c>
@@ -4293,28 +4314,28 @@
         <v>-9995</v>
       </c>
       <c r="E81" s="2">
+        <v>-8885</v>
+      </c>
+      <c r="F81" s="2">
         <v>-8888</v>
       </c>
-      <c r="F81" s="2">
-        <v>-8885</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H81" s="2">
+      <c r="H81" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I81" s="2">
         <v>-8887</v>
       </c>
-      <c r="I81" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J81" s="2">
+      <c r="J81" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K81" s="2">
         <v>-9998</v>
       </c>
-      <c r="K81" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>104</v>
       </c>
@@ -4325,14 +4346,11 @@
         <v>45</v>
       </c>
       <c r="E82" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H82" s="2" t="s">
         <v>45</v>
       </c>
@@ -4340,13 +4358,16 @@
         <v>45</v>
       </c>
       <c r="J82" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K82" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K82" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>106</v>
       </c>
@@ -4356,29 +4377,29 @@
       <c r="D83" s="2">
         <v>-9995</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F83" s="2">
         <v>-8888</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H83" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I83" s="2">
+      <c r="I83" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J83" s="2">
         <v>-9999</v>
       </c>
-      <c r="J83" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K83" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>107</v>
       </c>
@@ -4389,28 +4410,28 @@
         <v>-9995</v>
       </c>
       <c r="E84" s="2">
+        <v>-8885</v>
+      </c>
+      <c r="F84" s="2">
         <v>-8888</v>
       </c>
-      <c r="F84" s="2">
-        <v>-8885</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H84" s="2">
+      <c r="H84" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I84" s="2">
         <v>-8887</v>
       </c>
-      <c r="I84" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J84" s="2">
+      <c r="J84" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K84" s="2">
         <v>-9998</v>
       </c>
-      <c r="K84" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>108</v>
       </c>
@@ -4421,28 +4442,28 @@
         <v>-9995</v>
       </c>
       <c r="E85" s="2">
+        <v>-8885</v>
+      </c>
+      <c r="F85" s="2">
         <v>-8888</v>
       </c>
-      <c r="F85" s="2">
-        <v>-8885</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H85" s="2">
+      <c r="H85" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I85" s="2">
         <v>-8887</v>
       </c>
-      <c r="I85" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J85" s="2">
+      <c r="J85" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K85" s="2">
         <v>-9998</v>
       </c>
-      <c r="K85" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L85" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>109</v>
       </c>
@@ -4453,14 +4474,11 @@
         <v>45</v>
       </c>
       <c r="E86" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H86" s="2" t="s">
         <v>45</v>
       </c>
@@ -4468,13 +4486,16 @@
         <v>45</v>
       </c>
       <c r="J86" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K86" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K86" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L86" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>110</v>
       </c>
@@ -4484,29 +4505,29 @@
       <c r="D87" s="2">
         <v>-9995</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="2">
         <v>-8888</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H87" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I87" s="2">
+      <c r="I87" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J87" s="2">
         <v>-9999</v>
       </c>
-      <c r="J87" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K87" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L87" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>111</v>
       </c>
@@ -4517,28 +4538,28 @@
         <v>-9995</v>
       </c>
       <c r="E88" s="2">
+        <v>-8885</v>
+      </c>
+      <c r="F88" s="2">
         <v>-8888</v>
       </c>
-      <c r="F88" s="2">
-        <v>-8885</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H88" s="2">
+      <c r="H88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I88" s="2">
         <v>-8887</v>
       </c>
-      <c r="I88" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J88" s="2">
+      <c r="J88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K88" s="2">
         <v>-9998</v>
       </c>
-      <c r="K88" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L88" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>112</v>
       </c>
@@ -4549,28 +4570,28 @@
         <v>-9995</v>
       </c>
       <c r="E89" s="2">
+        <v>-8885</v>
+      </c>
+      <c r="F89" s="2">
         <v>-8888</v>
       </c>
-      <c r="F89" s="2">
-        <v>-8885</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H89" s="2">
+      <c r="H89" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I89" s="2">
         <v>-8887</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J89" s="2">
+      <c r="J89" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K89" s="2">
         <v>-9998</v>
       </c>
-      <c r="K89" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L89" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>48</v>
       </c>
@@ -4586,23 +4607,23 @@
       <c r="F90" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G90" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H90" s="2">
+      <c r="H90" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I90" s="2">
         <v>-8886</v>
       </c>
-      <c r="I90" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J90" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L90" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>115</v>
       </c>
@@ -4616,14 +4637,11 @@
         <v>45</v>
       </c>
       <c r="E91" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H91" s="2" t="s">
         <v>45</v>
       </c>
@@ -4636,8 +4654,11 @@
       <c r="K91" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L91" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>97</v>
       </c>
@@ -4653,23 +4674,23 @@
       <c r="F92" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G92" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H92" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I92" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I92" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J92" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L92" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>99</v>
       </c>
@@ -4685,23 +4706,23 @@
       <c r="F93" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G93" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H93" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I93" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I93" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J93" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L93" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>101</v>
       </c>
@@ -4717,23 +4738,23 @@
       <c r="F94" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G94" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H94" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I94" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J94" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L94" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>103</v>
       </c>
@@ -4749,23 +4770,23 @@
       <c r="F95" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G95" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H95" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I95" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I95" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J95" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L95" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>105</v>
       </c>
@@ -4781,19 +4802,19 @@
       <c r="F96" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G96" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H96" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I96" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I96" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J96" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K96" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L96" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>